<commit_message>
Revert back to previous time analysis stuff and add updated data to reflect analysis
</commit_message>
<xml_diff>
--- a/data/TimeComplexity - COW.xlsx
+++ b/data/TimeComplexity - COW.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbrib\OneDrive\Documents\College\The College of Wooster\Senior\I.S\Shapefile-Network-Navigator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbrib\OneDrive\Documents\College\The College of Wooster\Senior\I.S\Shapefile-Network-Navigator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_A105F5F4C51C08159223DC6D6F1DDA0E312B083C" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{1E922EC0-83AC-4A5E-9DE6-25A8AAA5213F}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="11_A105F5F4C51C08159223DC6D6F1DDA0E312B083C" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{4BF30CB2-2A44-4928-B925-A4FAF30B3324}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -849,8 +849,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1040,6 +1041,1786 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>Dijkstra!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time Elapsed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Dijkstra!$A$2:$A$99</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="98"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>676</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>841</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>961</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1089</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1156</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1225</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1296</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1369</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1444</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1521</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1681</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1764</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1849</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1936</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2116</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2209</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2401</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2601</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2704</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2809</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2916</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3025</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3136</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3249</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3364</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3481</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3721</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3844</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3969</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4225</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4356</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4489</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4624</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4761</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4900</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5041</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5184</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5329</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5476</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5625</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5776</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5929</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6084</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6241</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6561</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6724</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6889</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>7056</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>7225</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>7396</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>7569</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>7744</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>7921</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8100</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8281</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>8464</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8649</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>8836</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9025</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9216</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9409</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9604</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Dijkstra!$B$2:$B$99</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="98"/>
+                <c:pt idx="0">
+                  <c:v>0.174091100692749</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17187762260437009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17179203033447271</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1027257442474365</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1655991077423096</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16351318359375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.17159104347229001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8374662399291992E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.2189788818359375E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.2384395599365227E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.15805864334106451</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.562070846557617E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.15812158584594729</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.1914868354797363</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.150151252746582E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1941900253295898E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.1860809326171882E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.3802471160888672E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.9892196655273438E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.1960010528564453E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.68084716796875E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.8799982070922852E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.1953811645507813E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.6915798187255859E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.0875444412231449E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.4976253509521481E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.8969049453735352E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.201677322387695E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.886867523193359E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.4005899429321291E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.5957355499267582E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.0922908782958979E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.7925252914428711E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.7006158828735352E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.592350006103516E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.9222660064697266E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.899409294128418E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.40073299407959E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.5957355499267582E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.196599006652832E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.4959096908569339E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.9804916381835938E-3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.101207733154297E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7.9679489135742188E-3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.59149169921875E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.600241661071777E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>9.9725723266601563E-3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.89056396484375E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.295948028564453E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.5998125076293949E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.4919252395629883E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.8902778625488281E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>9.9697113037109375E-3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.297283172607422E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>7.9782009124755859E-3</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.5914201736450199E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.101398468017578E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>7.9782009124755859E-3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.500725746154785E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.5957355499267582E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.0968685150146479E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>8.9757442474365234E-3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.994729042053223E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.0919809341430661E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.9867630004882813E-3</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.001429557800293E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>7.9829692840576172E-3</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9.9713802337646484E-3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.9801807403564453E-3</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6.9816112518310547E-3</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.4958858489990229E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6.9823265075683594E-3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>8.9738368988037109E-3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.0018768310546884E-3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.0969638824462891E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.9779624938964844E-3</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8.0258846282958984E-3</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.9291591644287109E-3</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>8.975982666015625E-3</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>9.9651813507080078E-3</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>7.9565048217773438E-3</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.9786052703857422E-3</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6.9811344146728524E-3</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.9896965026855469E-3</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.0180168151855469E-3</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.9977302551269531E-3</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.0165863037109375E-3</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2.9923915863037109E-3</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>7.9805850982666016E-3</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6.9832801818847656E-3</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>6.969451904296875E-3</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.9935111999511719E-3</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>7.9708099365234375E-3</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.1968612670898439E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>6.9828033447265616E-3</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>7.0300102233886719E-3</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>8.0289840698242188E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-339D-42B9-B8DC-F7066AF316A3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="748320696"/>
+        <c:axId val="748322616"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="748320696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="748322616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="748322616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="748320696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ford Bellman'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time Elapsed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ford Bellman'!$A$2:$A$99</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="98"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>676</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>841</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>961</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1089</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1156</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1225</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1296</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1369</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1444</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1521</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1681</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1764</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1849</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1936</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2116</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2209</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2401</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2601</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2704</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2809</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2916</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3025</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3136</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3249</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3364</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3481</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3721</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3844</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3969</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4225</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4356</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4489</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4624</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4761</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4900</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5041</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5184</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5329</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5476</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5625</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5776</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5929</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6084</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6241</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6561</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6724</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6889</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>7056</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>7225</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>7396</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>7569</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>7744</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>7921</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8100</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8281</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>8464</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8649</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>8836</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9025</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9216</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9409</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9604</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ford Bellman'!$B$2:$B$99</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="98"/>
+                <c:pt idx="0">
+                  <c:v>1.0513250827789311</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0562376976013179</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.252671480178833</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.73004841804504395</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.159907341003418</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.093077421188354</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.116735458374023</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29609322547912598</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55378246307373047</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.16012787818908689</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.084102869033813</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1817777156829834</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.128656387329102</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.6569299697875977E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.233669519424438</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.30982375144958502</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.14760756492614749</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.2034566402435303</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.36901378631591802</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.28922700881958008</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.2223620414733887</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.3780362606048584</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.34907984733581537</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.2154271602630615</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.1077532768249512</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.18653726577758789</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.14860343933105469</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.17353105545043951</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.4750661849975586E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.17059111595153811</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.6774587631225586E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.3762397766113281E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.3877582550048828E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.17054247856140139</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.4695091247558594E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.6796035766601563E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.1874866485595703E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.110706090927124</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.8785896301269531E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.7735881805419922E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.7803869247436523E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8.3829164505004883E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.7931451797485352E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.6781282424926758E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.8907527923583977E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8.48236083984375E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.10367751121521</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6.5874338150024414E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.1057186126708984</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7.9785346984863281E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>9.4704627990722656E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.9855241775512702E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.1067142486572266</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6.0831546783447273E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6.9805383682250977E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.0898323059082031E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>9.2750310897827148E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.9836626052856452E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.3923616409301758E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>8.1734418869018555E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>8.6768150329589844E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>7.3804855346679688E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.8868656158447273E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>7.3801755905151367E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.3828706741333008E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.794338226318359E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.288935661315918E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.889775276184082E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5.8839321136474609E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.994776725769043E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.9890289306640618E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.8686456680297852E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>9.4795942306518555E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.7871112823486328E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.9871692657470703E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6.4826726913452148E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.89404296875E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4.4872045516967773E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.9893388748168952E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.3883562088012702E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4.2928695678710938E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.9893865585327148E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.8909902572631843E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.3883085250854492E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.0963430404663089E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.2887449264526367E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2.093195915222168E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4.687952995300293E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2.397608757019043E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.8896083831787109E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.5892496109008789E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.9896965026855469E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>4.9863576889038093E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3.9893150329589837E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4.3883800506591797E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4.4878959655761719E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4.383540153503418E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.8896083831787109E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ADEA-4098-BA04-01A68360718E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="660730296"/>
+        <c:axId val="660726456"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="660730296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="660726456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="660726456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="660730296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>'A-star'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1739,8 +3520,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1876,7 +3658,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1891,6 +3673,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Algorithms</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Time Elapsed</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3959,8 +5770,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -4246,6 +6058,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -5323,6 +7215,1082 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5905,6 +8873,88 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EE6658D-8B6F-47F3-AD26-5AE3D47E151D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD057398-A26D-4FE3-8A56-EB64E1FC861B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -5942,20 +8992,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:colOff>561974</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>80961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6306,8 +9356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:B99"/>
+    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7119,7 +10169,7 @@
   <dimension ref="A1:B99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B99"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7922,6 +10972,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7930,7 +10981,7 @@
   <dimension ref="A1:B99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8733,6 +11784,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9552,8 +12604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ECFE7FE-B21B-41A2-811C-CC1969AB8261}">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix node duplicates and update time analysis
</commit_message>
<xml_diff>
--- a/data/TimeComplexity - COW.xlsx
+++ b/data/TimeComplexity - COW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbrib\OneDrive\Documents\College\The College of Wooster\Senior\I.S\Shapefile-Network-Navigator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="11_A105F5F4C51C08159223DC6D6F1DDA0E312B083C" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{4BF30CB2-2A44-4928-B925-A4FAF30B3324}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="11_A105F5F4C51C08159223DC6D6F1DDA0E312B083C" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{7AAFE804-94F2-49AD-901B-09AFDBB9C3E6}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="time and grid size" sheetId="1" r:id="rId1"/>
@@ -1740,8 +1740,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2630,8 +2631,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -3732,7 +3734,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.1490109640885347E-2"/>
+          <c:y val="0.10177210930612283"/>
+          <c:w val="0.94162720209028772"/>
+          <c:h val="0.85001118605028336"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -8835,13 +8847,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>80961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>268432</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>103908</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9004,8 +9016,8 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9356,7 +9368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -12604,8 +12616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ECFE7FE-B21B-41A2-811C-CC1969AB8261}">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>